<commit_message>
Add wards and subwards
</commit_message>
<xml_diff>
--- a/XForms/waste_collection.xlsx
+++ b/XForms/waste_collection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="336">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -90,39 +90,45 @@
     <t xml:space="preserve">minimal</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one wards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jina la Kata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which ward in lower Msimbazi ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kata gani huko Msimbazi ya chini?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixme: I need this list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one subward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-ward name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jina ndogo la Kata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which sub-wards in lower Msimbazi ?</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ward name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jina la Kata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which ward in lower Msimbazi ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kata gani huko Msimbazi ya chini?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixme: I need this list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub-ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub-ward name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jina ndogo la Kata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which sub-wards in lower Msimbazi ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">mtaa</t>
   </si>
   <si>
@@ -949,6 +955,72 @@
   </si>
   <si>
     <t xml:space="preserve">waste management services are poor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bunju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bunju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kinondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mji_mpya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mji Mpya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mbopo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mbopo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mabwepande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mabwepande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magharibi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magharibi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msimbazi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Msimbazi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mashariki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mashariki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matumbi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matumbi</t>
   </si>
   <si>
     <t xml:space="preserve">form_id</t>
@@ -968,7 +1040,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1063,6 +1135,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -1139,7 +1216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1272,11 +1349,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1303,8 +1388,8 @@
   </sheetPr>
   <dimension ref="A1:AC74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1499,22 +1584,22 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>28</v>
@@ -1525,19 +1610,19 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>21</v>
@@ -1545,7 +1630,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E15" s="9"/>
     </row>
@@ -1554,7 +1639,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>18</v>
@@ -1565,21 +1650,21 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>21</v>
@@ -1587,16 +1672,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>21</v>
@@ -1604,16 +1689,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>21</v>
@@ -1621,16 +1706,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>21</v>
@@ -1638,19 +1723,19 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>21</v>
@@ -1658,7 +1743,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,7 +1751,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>18</v>
@@ -1677,24 +1762,24 @@
         <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>21</v>
@@ -1702,16 +1787,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>21</v>
@@ -1719,16 +1804,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>21</v>
@@ -1736,19 +1821,19 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>21</v>
@@ -1756,16 +1841,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>21</v>
@@ -1773,19 +1858,19 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H33" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>21</v>
@@ -1793,7 +1878,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1801,7 +1886,7 @@
         <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
@@ -1812,7 +1897,7 @@
         <v>19</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>21</v>
@@ -1820,17 +1905,17 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D39" s="0"/>
       <c r="H39" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>21</v>
@@ -1838,16 +1923,16 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>21</v>
@@ -1855,17 +1940,17 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D41" s="0"/>
       <c r="H41" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>21</v>
@@ -1873,16 +1958,16 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>21</v>
@@ -1890,17 +1975,17 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D43" s="0"/>
       <c r="H43" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>21</v>
@@ -1908,16 +1993,16 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H44" s="0"/>
       <c r="J44" s="1" t="s">
@@ -1926,17 +2011,17 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D45" s="0"/>
       <c r="H45" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>21</v>
@@ -1944,16 +2029,16 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>21</v>
@@ -1961,7 +2046,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,7 +2054,7 @@
         <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>18</v>
@@ -1980,7 +2065,7 @@
         <v>19</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>21</v>
@@ -1988,16 +2073,16 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>21</v>
@@ -2005,19 +2090,19 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>21</v>
@@ -2025,19 +2110,19 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>21</v>
@@ -2045,16 +2130,16 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>21</v>
@@ -2062,16 +2147,16 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>21</v>
@@ -2079,19 +2164,19 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>21</v>
@@ -2099,16 +2184,16 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>21</v>
@@ -2116,19 +2201,19 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>21</v>
@@ -2136,7 +2221,7 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2229,7 @@
         <v>16</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>18</v>
@@ -2155,7 +2240,7 @@
         <v>19</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>21</v>
@@ -2163,16 +2248,16 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>21</v>
@@ -2180,16 +2265,16 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>21</v>
@@ -2197,16 +2282,16 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>21</v>
@@ -2214,16 +2299,16 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>21</v>
@@ -2231,7 +2316,7 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2239,41 +2324,41 @@
         <v>16</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C69" s="12"/>
       <c r="E69" s="13"/>
       <c r="J69" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="70" s="16" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G70" s="16" t="n">
         <v>1.5</v>
       </c>
       <c r="H70" s="17"/>
       <c r="J70" s="16" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="18" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D71" s="18"/>
       <c r="E71" s="20"/>
@@ -2306,13 +2391,13 @@
     </row>
     <row r="72" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="21" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D72" s="21"/>
       <c r="E72" s="23"/>
@@ -2324,7 +2409,7 @@
         <v>21</v>
       </c>
       <c r="K72" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L72" s="27"/>
       <c r="M72" s="27"/>
@@ -2347,13 +2432,13 @@
     </row>
     <row r="73" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D73" s="21"/>
       <c r="E73" s="23"/>
@@ -2365,7 +2450,7 @@
         <v>21</v>
       </c>
       <c r="K73" s="26" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="L73" s="27"/>
       <c r="M73" s="27"/>
@@ -2388,7 +2473,7 @@
     </row>
     <row r="74" s="16" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B74" s="18"/>
       <c r="C74" s="18"/>
@@ -2435,10 +2520,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="1" sqref="H43 C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B127" activeCellId="0" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2453,7 +2538,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -2467,947 +2552,947 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3415,46 +3500,159 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="33"/>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B122" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="C122" s="34" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B123" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C123" s="34" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B124" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="C124" s="34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B125" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="C125" s="34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B126" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="C126" s="34" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3476,7 +3674,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="H43 B3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3485,40 +3683,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
+      <c r="A1" s="35" t="s">
+        <v>333</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="n">
+      <c r="A2" s="37" t="n">
         <f aca="true">NOW()</f>
-        <v>44276.7358589667</v>
+        <v>44276.755504064</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>311</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>